<commit_message>
Disabled button when text field is empty.
</commit_message>
<xml_diff>
--- a/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
+++ b/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Personal Projects\StarWarsCharacterGuessingGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24755C44-F1FD-400F-A689-1A1C18C3CEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBE7C35-BC99-402D-85F8-9943C769001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>Gender/Droid Type</t>
   </si>
   <si>
-    <t>First on Screen Appearance</t>
-  </si>
-  <si>
     <t>Birth Year</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>https://media.vogue.fr/photos/606dca7e47f477da2ff11fcf/1:1/w_2032,h_2032,c_limit/010_A7A08C89_416.jpg</t>
+  </si>
+  <si>
+    <t>First Screen Appearance</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,97 +1009,97 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor tweaks (removed unused imports, added to TODO list).
</commit_message>
<xml_diff>
--- a/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
+++ b/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Personal Projects\StarWarsCharacterGuessingGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBE7C35-BC99-402D-85F8-9943C769001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{681A6864-92C2-43A0-B190-18093A909FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -120,6 +120,66 @@
   </si>
   <si>
     <t>First Screen Appearance</t>
+  </si>
+  <si>
+    <t>R2-D2</t>
+  </si>
+  <si>
+    <t>Droid</t>
+  </si>
+  <si>
+    <t>Astromech</t>
+  </si>
+  <si>
+    <t>~32 BBY</t>
+  </si>
+  <si>
+    <t>Naboo</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/R2-D2</t>
+  </si>
+  <si>
+    <t>https://pyxis.nymag.com/v1/imgs/7ef/846/3245bc42a87b290d806985f75dc6e7bd4a-28-r2-d2.rsquare.w330.jpg</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>41 BBY</t>
+  </si>
+  <si>
+    <t>The Mandalorian (Season 1, 2019)</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Grogu</t>
+  </si>
+  <si>
+    <t>Grogu (The Child)</t>
+  </si>
+  <si>
+    <t>https://pyxis.nymag.com/v1/imgs/99e/6f5/6eed622d1b1b0a77caad3e658d61630b76-baby-yoda.rsquare.w700.jpg</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Maul</t>
+  </si>
+  <si>
+    <t>Zabrak</t>
+  </si>
+  <si>
+    <t>54 BBY</t>
+  </si>
+  <si>
+    <t>Dathomir</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/cc/bb/02/ccbb029fca3b6bf6256b49acc110a200.jpg</t>
+  </si>
+  <si>
+    <t>Epsiode I: The Phantom Menace (1999)</t>
+  </si>
+  <si>
+    <t>Darth Maul</t>
   </si>
 </sst>
 </file>
@@ -979,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,8 +1052,8 @@
     <col min="3" max="3" width="24" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="52.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="45.7109375" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -1103,7 +1163,82 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="3"/>
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1113,8 +1248,14 @@
     <hyperlink ref="H2" r:id="rId4" xr:uid="{99621230-DD10-401C-BDB8-AD114CDE70A5}"/>
     <hyperlink ref="H4" r:id="rId5" xr:uid="{5EF7C6C9-17A2-42EE-9AB5-62158257BA50}"/>
     <hyperlink ref="H3" r:id="rId6" xr:uid="{58F0C59A-D662-47F1-956B-645051D00A7D}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{B31B78B6-6D5E-4883-861F-B2A6C483A498}"/>
+    <hyperlink ref="H5" r:id="rId8" xr:uid="{3FC1F4A8-DCCE-4B2A-8BB9-867CCA962E25}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{F6B5FACF-1701-4387-99D1-CFB411CE90F5}"/>
+    <hyperlink ref="H6" r:id="rId10" xr:uid="{D29EA736-8196-49D6-AD8A-EB01C3A7F191}"/>
+    <hyperlink ref="G7" r:id="rId11" xr:uid="{B51D34D1-860A-4242-B462-8C84CC3F7A5C}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{DB0C3C41-5E25-4D7A-8DFE-43A7807436FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added comments for the first half.
</commit_message>
<xml_diff>
--- a/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
+++ b/out/production/StarWarsCharacterGuessingGame/data/sw_character_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Personal Projects\StarWarsCharacterGuessingGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADC4A1B2-A7A9-4B20-A116-1CADC5320CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6944112F-E413-46F4-8D17-E8938CB95627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -297,6 +297,54 @@
   </si>
   <si>
     <t>https://winteriscoming.net/files/image-exchange/2018/08/ie_61486-150x150.jpeg</t>
+  </si>
+  <si>
+    <t>15 ABY</t>
+  </si>
+  <si>
+    <t>Jakku</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Rey_Skywalker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rey </t>
+  </si>
+  <si>
+    <t>Mon Calamari</t>
+  </si>
+  <si>
+    <t>Dac</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Gial_Ackbar/Legends</t>
+  </si>
+  <si>
+    <t>Lando Calrissian</t>
+  </si>
+  <si>
+    <t>31 BBY</t>
+  </si>
+  <si>
+    <t>Socorro</t>
+  </si>
+  <si>
+    <t>Episode VII: The Force Awakens (2015)</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Lando_Calrissian/Legends</t>
+  </si>
+  <si>
+    <t>https://cdn.vox-cdn.com/thumbor/Iygx7I0plaTWBYzEuzso_zYEYWg=/1400x1400/filters:format(jpeg)/cdn.vox-cdn.com/uploads/chorus_asset/file/6332771/Lando-Calrissian_a679fe1e.0.jpeg</t>
+  </si>
+  <si>
+    <t>Admiral Gial Ackbar</t>
+  </si>
+  <si>
+    <t>https://pyxis.nymag.com/v1/imgs/854/921/9242868f6d9e25cfa955b32c070e3cbb7c-13-the-last-jedi-rey-2.rsquare.w700.jpg</t>
+  </si>
+  <si>
+    <t>https://pyxis.nymag.com/v1/imgs/5fd/b4c/08e5eaa592aaf4c45ca001b680bb827ae7-13-ackbar.rsquare.w700.jpg</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,6 +1612,84 @@
       </c>
       <c r="H15" s="3" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1595,8 +1721,12 @@
     <hyperlink ref="H15" r:id="rId25" xr:uid="{20232027-9225-4818-AF50-A85197C42B88}"/>
     <hyperlink ref="G14" r:id="rId26" xr:uid="{49919947-F803-401D-8083-0E3B8B97A385}"/>
     <hyperlink ref="H14" r:id="rId27" xr:uid="{8E6D595D-7CA5-4DCD-9493-47213BF15AC6}"/>
+    <hyperlink ref="G16" r:id="rId28" xr:uid="{5D19242D-E59E-4A23-830C-76BDB589688C}"/>
+    <hyperlink ref="G18" r:id="rId29" xr:uid="{D56E8AA5-8B05-46FB-9CED-0BF6DA88621F}"/>
+    <hyperlink ref="H16" r:id="rId30" xr:uid="{34A50A88-CAD6-4519-8850-CB17A730C8A6}"/>
+    <hyperlink ref="H17" r:id="rId31" xr:uid="{F6AFD7C1-7EA3-42C6-A7DC-4AE07F0A7FEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>